<commit_message>
Total of 6 TCs. --> in LoginTest.java - LoginWithAnalyzer - LoginWithIndividual - LoginWithUser - LoginWithSchemaManager - LoginWithUserManager - LoginWithSuperUser
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Variable</t>
   </si>
@@ -20,6 +20,18 @@
     <t>Supported Browser Types</t>
   </si>
   <si>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
+  </si>
+  <si>
     <t>Data1</t>
   </si>
   <si>
@@ -35,18 +47,6 @@
     <t>Data5</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>Data6</t>
   </si>
   <si>
@@ -98,6 +98,15 @@
     <t>AbdelsalamSchemaManager</t>
   </si>
   <si>
+    <t>AbdelsalamUser</t>
+  </si>
+  <si>
+    <t>AbdelsalamUserManager</t>
+  </si>
+  <si>
+    <t>AbdelsalamSuper</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
@@ -108,6 +117,15 @@
   </si>
   <si>
     <t>AbdelsalamSchemaManager1</t>
+  </si>
+  <si>
+    <t>AbdelsalamUser1</t>
+  </si>
+  <si>
+    <t>AbdelsalamUserManager1</t>
+  </si>
+  <si>
+    <t>AbdelsalamSuper1</t>
   </si>
 </sst>
 </file>
@@ -184,11 +202,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -247,35 +265,35 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -412,9 +430,15 @@
       <c r="D8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="E8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -437,9 +461,15 @@
       <c r="D9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="E9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -451,20 +481,26 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+        <v>34</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -1492,79 +1528,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
LoginTest.java --> Added a new script for TC checking schema manager permissions.
Skeleton.java --> Added a new function to click on elements in the side
menu.

Updated Excel file in Security folder.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security/TestData.xlsx
@@ -12,14 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+  <si>
+    <t>Supported Browser Types</t>
+  </si>
   <si>
     <t>Variable</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
-  </si>
-  <si>
     <t>MozillaFirefox</t>
   </si>
   <si>
@@ -77,6 +77,36 @@
     <t>security/users</t>
   </si>
   <si>
+    <t>URL_data_dataSources</t>
+  </si>
+  <si>
+    <t>datasources/datasource</t>
+  </si>
+  <si>
+    <t>URL_data_dataFiles</t>
+  </si>
+  <si>
+    <t>datasources/dataFiles</t>
+  </si>
+  <si>
+    <t>URL_schemas_schemaList</t>
+  </si>
+  <si>
+    <t>schemas/schema-list</t>
+  </si>
+  <si>
+    <t>URL_scheduler_schemas</t>
+  </si>
+  <si>
+    <t>schedulers/scheduler-schemas</t>
+  </si>
+  <si>
+    <t>URL_scheduler_dashboards</t>
+  </si>
+  <si>
+    <t>schedulers/scheduler-dashboards</t>
+  </si>
+  <si>
     <t>User Credentials Analyzer</t>
   </si>
   <si>
@@ -126,13 +156,64 @@
   </si>
   <si>
     <t>AbdelsalamSuper1</t>
+  </si>
+  <si>
+    <t>TC008 - Create DataSource</t>
+  </si>
+  <si>
+    <t>DataSourceType</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>DataSourceUsername</t>
+  </si>
+  <si>
+    <t>salesdb</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>DataSourcePassword</t>
+  </si>
+  <si>
+    <t>r00tmy$Ql</t>
+  </si>
+  <si>
+    <t>DataSourceConnectionPool</t>
+  </si>
+  <si>
+    <t>DataSourceConnectionString</t>
+  </si>
+  <si>
+    <t>jdbc:oracle:thin:@qa.incorta.com:1521:xe</t>
+  </si>
+  <si>
+    <t>jdbc:mysql://qa.incorta.com:3306/salesdb</t>
+  </si>
+  <si>
+    <t>TC011 - Add DataSource to Schema using Wizard</t>
+  </si>
+  <si>
+    <t>DatabaseName</t>
+  </si>
+  <si>
+    <t>DatabaseTableName</t>
+  </si>
+  <si>
+    <t>sales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -151,6 +232,10 @@
       <name val="Calibri"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -172,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border/>
     <border>
       <left/>
@@ -194,11 +279,14 @@
       <top/>
       <bottom/>
     </border>
+    <border>
+      <bottom/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -222,11 +310,26 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -266,7 +369,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -402,128 +505,572 @@
       <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
+      <c r="B7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
+      <c r="B8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+    </row>
+    <row r="11" ht="13.5" customHeight="1">
+      <c r="A11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+    </row>
+    <row r="12" ht="13.5" customHeight="1">
+      <c r="A12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+    </row>
+    <row r="13" ht="13.5" customHeight="1">
+      <c r="A13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="C13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" ht="13.5" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="B14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="C14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="D14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="E14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
     </row>
-    <row r="11" ht="13.5" customHeight="1"/>
-    <row r="12" ht="13.5" customHeight="1"/>
-    <row r="13" ht="13.5" customHeight="1"/>
-    <row r="14" ht="13.5" customHeight="1"/>
-    <row r="15" ht="13.5" customHeight="1"/>
-    <row r="16" ht="13.5" customHeight="1"/>
-    <row r="17" ht="13.5" customHeight="1"/>
-    <row r="18" ht="13.5" customHeight="1"/>
-    <row r="19" ht="13.5" customHeight="1"/>
-    <row r="20" ht="13.5" customHeight="1"/>
-    <row r="21" ht="13.5" customHeight="1"/>
-    <row r="22" ht="13.5" customHeight="1"/>
-    <row r="23" ht="13.5" customHeight="1"/>
-    <row r="24" ht="13.5" customHeight="1"/>
+    <row r="15" ht="13.5" customHeight="1">
+      <c r="A15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+    </row>
+    <row r="16" ht="13.5" customHeight="1">
+      <c r="A16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+    </row>
+    <row r="17" ht="13.5" customHeight="1">
+      <c r="A17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+    </row>
+    <row r="18" ht="13.5" customHeight="1">
+      <c r="A18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+    </row>
+    <row r="19" ht="13.5" customHeight="1">
+      <c r="A19" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+    </row>
+    <row r="20" ht="13.5" customHeight="1">
+      <c r="A20" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="9">
+        <v>30.0</v>
+      </c>
+      <c r="C20" s="9">
+        <v>30.0</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+    </row>
+    <row r="21" ht="13.5" customHeight="1">
+      <c r="A21" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+    </row>
+    <row r="22" ht="13.5" customHeight="1">
+      <c r="A22" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+    </row>
+    <row r="23" ht="13.5" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+    </row>
+    <row r="24" ht="13.5" customHeight="1">
+      <c r="A24" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="10"/>
+    </row>
     <row r="25" ht="13.5" customHeight="1"/>
     <row r="26" ht="13.5" customHeight="1"/>
     <row r="27" ht="13.5" customHeight="1"/>
@@ -620,11 +1167,11 @@
     <row r="118" ht="13.5" customHeight="1"/>
     <row r="119" ht="13.5" customHeight="1"/>
     <row r="120" ht="13.5" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="121" ht="13.5" customHeight="1"/>
+    <row r="122" ht="13.5" customHeight="1"/>
+    <row r="123" ht="13.5" customHeight="1"/>
+    <row r="124" ht="13.5" customHeight="1"/>
+    <row r="125" ht="13.5" customHeight="1"/>
     <row r="126" ht="15.75" customHeight="1"/>
     <row r="127" ht="15.75" customHeight="1"/>
     <row r="128" ht="15.75" customHeight="1"/>
@@ -1500,10 +2047,17 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -1529,7 +2083,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>

</xml_diff>

<commit_message>
Fix corrupted security Test Data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>Supported Browser Types</t>
   </si>
@@ -207,18 +207,6 @@
   </si>
   <si>
     <t>sales</t>
-  </si>
-  <si>
-    <t>TC_C469 - Add Roles To Group</t>
-  </si>
-  <si>
-    <t>GroupRoles</t>
-  </si>
-  <si>
-    <t>Analyze User</t>
-  </si>
-  <si>
-    <t>Schema Manager</t>
   </si>
 </sst>
 </file>
@@ -298,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -343,9 +331,6 @@
     <xf borderId="4" fillId="3" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1052,7 +1037,7 @@
       <c r="Y23" s="10"/>
       <c r="Z23" s="10"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="11" t="s">
         <v>63</v>
       </c>
@@ -1086,70 +1071,8 @@
       <c r="Y24" s="10"/>
       <c r="Z24" s="10"/>
     </row>
-    <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
-      <c r="V25" s="10"/>
-      <c r="W25" s="10"/>
-      <c r="X25" s="10"/>
-      <c r="Y25" s="10"/>
-      <c r="Z25" s="10"/>
-    </row>
-    <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
-      <c r="T26" s="10"/>
-      <c r="U26" s="10"/>
-      <c r="V26" s="10"/>
-      <c r="W26" s="10"/>
-      <c r="X26" s="10"/>
-      <c r="Y26" s="10"/>
-      <c r="Z26" s="10"/>
-    </row>
+    <row r="25" ht="13.5" customHeight="1"/>
+    <row r="26" ht="13.5" customHeight="1"/>
     <row r="27" ht="13.5" customHeight="1"/>
     <row r="28" ht="13.5" customHeight="1"/>
     <row r="29" ht="13.5" customHeight="1"/>
@@ -2130,12 +2053,11 @@
     <row r="1004" ht="15.75" customHeight="1"/>
     <row r="1005" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Fix failing issues at users\groups test
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security/TestData.xlsx
@@ -12,12 +12,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+  <si>
+    <t>Variable</t>
+  </si>
   <si>
     <t>Supported Browser Types</t>
   </si>
   <si>
-    <t>Variable</t>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>Data5</t>
+  </si>
+  <si>
+    <t>Data6</t>
+  </si>
+  <si>
+    <t>Data7</t>
   </si>
   <si>
     <t>MozillaFirefox</t>
@@ -32,24 +53,6 @@
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
-    <t>Data5</t>
-  </si>
-  <si>
-    <t>Data6</t>
-  </si>
-  <si>
     <t>URLs</t>
   </si>
   <si>
@@ -137,6 +140,9 @@
     <t>AbdelsalamSuper</t>
   </si>
   <si>
+    <t>admin</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
@@ -158,7 +164,7 @@
     <t>AbdelsalamSuper1</t>
   </si>
   <si>
-    <t>TC008 - Create DataSource</t>
+    <t>Create DataSource</t>
   </si>
   <si>
     <t>DataSourceType</t>
@@ -197,7 +203,7 @@
     <t>jdbc:mysql://qa.incorta.com:3306/salesdb</t>
   </si>
   <si>
-    <t>TC011 - Add DataSource to Schema using Wizard</t>
+    <t>Add DataSource to Schema using Wizard</t>
   </si>
   <si>
     <t>DatabaseName</t>
@@ -207,13 +213,40 @@
   </si>
   <si>
     <t>sales</t>
+  </si>
+  <si>
+    <t>Add Roles To Group</t>
+  </si>
+  <si>
+    <t>GroupRoles</t>
+  </si>
+  <si>
+    <t>Analyze User</t>
+  </si>
+  <si>
+    <t>Schema Manager</t>
+  </si>
+  <si>
+    <t>Impersonation</t>
+  </si>
+  <si>
+    <t>ImpersonationUserName</t>
+  </si>
+  <si>
+    <t>Analyzer User</t>
+  </si>
+  <si>
+    <t>ImpersonationMessage</t>
+  </si>
+  <si>
+    <t>You’re temporarily logged in as Analyzer User. To switch back to your account, click on the icon at the bottom left of your screen.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -236,6 +269,9 @@
       <sz val="11.0"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <color rgb="FF454545"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -257,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border/>
     <border>
       <left/>
@@ -279,22 +315,19 @@
       <top/>
       <bottom/>
     </border>
-    <border>
-      <bottom/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -303,7 +336,6 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -316,20 +348,20 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -364,814 +396,769 @@
     <col customWidth="1" min="5" max="6" width="28.29"/>
     <col customWidth="1" min="7" max="7" width="28.86"/>
     <col customWidth="1" min="8" max="15" width="8.57"/>
-    <col customWidth="1" min="16" max="26" width="8.71"/>
+    <col customWidth="1" min="16" max="17" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
+      <c r="B4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="B5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="B6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10"/>
+      <c r="B7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
+      <c r="B8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="10"/>
+      <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
+      <c r="B10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="10"/>
+      <c r="B11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="12" t="s">
-        <v>31</v>
+      <c r="A12" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="C14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="D14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="E14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="F14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
+      <c r="G14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="13" t="s">
+      <c r="A15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="14" t="s">
-        <v>48</v>
+      <c r="A16" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="10"/>
+      <c r="B17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
+      <c r="B18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="10"/>
-      <c r="Z19" s="10"/>
+      <c r="C19" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="9">
+      <c r="A20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="8">
         <v>30.0</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>30.0</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="10"/>
-      <c r="Z20" s="10"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="11" t="s">
+      <c r="A21" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
-      <c r="V21" s="10"/>
-      <c r="W21" s="10"/>
-      <c r="X21" s="10"/>
-      <c r="Y21" s="10"/>
-      <c r="Z21" s="10"/>
+      <c r="B21" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="14" t="s">
-        <v>61</v>
+      <c r="A22" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
-      <c r="W22" s="10"/>
-      <c r="X22" s="10"/>
-      <c r="Y22" s="10"/>
-      <c r="Z22" s="10"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="10"/>
-      <c r="Y23" s="10"/>
-      <c r="Z23" s="10"/>
+      <c r="A23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="10"/>
-      <c r="U24" s="10"/>
-      <c r="V24" s="10"/>
-      <c r="W24" s="10"/>
-      <c r="X24" s="10"/>
-      <c r="Y24" s="10"/>
-      <c r="Z24" s="10"/>
-    </row>
-    <row r="25" ht="13.5" customHeight="1"/>
-    <row r="26" ht="13.5" customHeight="1"/>
-    <row r="27" ht="13.5" customHeight="1"/>
-    <row r="28" ht="13.5" customHeight="1"/>
-    <row r="29" ht="13.5" customHeight="1"/>
-    <row r="30" ht="13.5" customHeight="1"/>
-    <row r="31" ht="13.5" customHeight="1"/>
-    <row r="32" ht="13.5" customHeight="1"/>
-    <row r="33" ht="13.5" customHeight="1"/>
-    <row r="34" ht="13.5" customHeight="1"/>
-    <row r="35" ht="13.5" customHeight="1"/>
-    <row r="36" ht="13.5" customHeight="1"/>
-    <row r="37" ht="13.5" customHeight="1"/>
-    <row r="38" ht="13.5" customHeight="1"/>
-    <row r="39" ht="13.5" customHeight="1"/>
-    <row r="40" ht="13.5" customHeight="1"/>
-    <row r="41" ht="13.5" customHeight="1"/>
-    <row r="42" ht="13.5" customHeight="1"/>
-    <row r="43" ht="13.5" customHeight="1"/>
-    <row r="44" ht="13.5" customHeight="1"/>
-    <row r="45" ht="13.5" customHeight="1"/>
-    <row r="46" ht="13.5" customHeight="1"/>
-    <row r="47" ht="13.5" customHeight="1"/>
-    <row r="48" ht="13.5" customHeight="1"/>
-    <row r="49" ht="13.5" customHeight="1"/>
-    <row r="50" ht="13.5" customHeight="1"/>
-    <row r="51" ht="13.5" customHeight="1"/>
-    <row r="52" ht="13.5" customHeight="1"/>
-    <row r="53" ht="13.5" customHeight="1"/>
-    <row r="54" ht="13.5" customHeight="1"/>
-    <row r="55" ht="13.5" customHeight="1"/>
-    <row r="56" ht="13.5" customHeight="1"/>
-    <row r="57" ht="13.5" customHeight="1"/>
-    <row r="58" ht="13.5" customHeight="1"/>
-    <row r="59" ht="13.5" customHeight="1"/>
-    <row r="60" ht="13.5" customHeight="1"/>
-    <row r="61" ht="13.5" customHeight="1"/>
-    <row r="62" ht="13.5" customHeight="1"/>
-    <row r="63" ht="13.5" customHeight="1"/>
-    <row r="64" ht="13.5" customHeight="1"/>
-    <row r="65" ht="13.5" customHeight="1"/>
-    <row r="66" ht="13.5" customHeight="1"/>
-    <row r="67" ht="13.5" customHeight="1"/>
-    <row r="68" ht="13.5" customHeight="1"/>
-    <row r="69" ht="13.5" customHeight="1"/>
-    <row r="70" ht="13.5" customHeight="1"/>
-    <row r="71" ht="13.5" customHeight="1"/>
-    <row r="72" ht="13.5" customHeight="1"/>
-    <row r="73" ht="13.5" customHeight="1"/>
-    <row r="74" ht="13.5" customHeight="1"/>
-    <row r="75" ht="13.5" customHeight="1"/>
-    <row r="76" ht="13.5" customHeight="1"/>
-    <row r="77" ht="13.5" customHeight="1"/>
-    <row r="78" ht="13.5" customHeight="1"/>
-    <row r="79" ht="13.5" customHeight="1"/>
-    <row r="80" ht="13.5" customHeight="1"/>
-    <row r="81" ht="13.5" customHeight="1"/>
-    <row r="82" ht="13.5" customHeight="1"/>
-    <row r="83" ht="13.5" customHeight="1"/>
-    <row r="84" ht="13.5" customHeight="1"/>
-    <row r="85" ht="13.5" customHeight="1"/>
-    <row r="86" ht="13.5" customHeight="1"/>
-    <row r="87" ht="13.5" customHeight="1"/>
-    <row r="88" ht="13.5" customHeight="1"/>
-    <row r="89" ht="13.5" customHeight="1"/>
-    <row r="90" ht="13.5" customHeight="1"/>
-    <row r="91" ht="13.5" customHeight="1"/>
-    <row r="92" ht="13.5" customHeight="1"/>
-    <row r="93" ht="13.5" customHeight="1"/>
-    <row r="94" ht="13.5" customHeight="1"/>
-    <row r="95" ht="13.5" customHeight="1"/>
-    <row r="96" ht="13.5" customHeight="1"/>
-    <row r="97" ht="13.5" customHeight="1"/>
-    <row r="98" ht="13.5" customHeight="1"/>
-    <row r="99" ht="13.5" customHeight="1"/>
-    <row r="100" ht="13.5" customHeight="1"/>
-    <row r="101" ht="13.5" customHeight="1"/>
-    <row r="102" ht="13.5" customHeight="1"/>
-    <row r="103" ht="13.5" customHeight="1"/>
-    <row r="104" ht="13.5" customHeight="1"/>
-    <row r="105" ht="13.5" customHeight="1"/>
-    <row r="106" ht="13.5" customHeight="1"/>
-    <row r="107" ht="13.5" customHeight="1"/>
-    <row r="108" ht="13.5" customHeight="1"/>
-    <row r="109" ht="13.5" customHeight="1"/>
-    <row r="110" ht="13.5" customHeight="1"/>
-    <row r="111" ht="13.5" customHeight="1"/>
-    <row r="112" ht="13.5" customHeight="1"/>
-    <row r="113" ht="13.5" customHeight="1"/>
-    <row r="114" ht="13.5" customHeight="1"/>
-    <row r="115" ht="13.5" customHeight="1"/>
-    <row r="116" ht="13.5" customHeight="1"/>
-    <row r="117" ht="13.5" customHeight="1"/>
-    <row r="118" ht="13.5" customHeight="1"/>
-    <row r="119" ht="13.5" customHeight="1"/>
-    <row r="120" ht="13.5" customHeight="1"/>
-    <row r="121" ht="13.5" customHeight="1"/>
-    <row r="122" ht="13.5" customHeight="1"/>
-    <row r="123" ht="13.5" customHeight="1"/>
-    <row r="124" ht="13.5" customHeight="1"/>
-    <row r="125" ht="13.5" customHeight="1"/>
+      <c r="A24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+    </row>
+    <row r="25" ht="13.5" customHeight="1">
+      <c r="A25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="13"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
     <row r="126" ht="15.75" customHeight="1"/>
     <row r="127" ht="15.75" customHeight="1"/>
     <row r="128" ht="15.75" customHeight="1"/>
@@ -2047,17 +2034,14 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
-    <row r="1005" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A27:C27"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2078,83 +2062,82 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="26.29"/>
     <col customWidth="1" min="2" max="11" width="8.57"/>
-    <col customWidth="1" min="12" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add all analyzer TCs
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security/TestData.xlsx
@@ -12,12 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
+  <si>
+    <t>Supported Browser Types</t>
+  </si>
   <si>
     <t>Variable</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
   </si>
   <si>
     <t>Data1</t>
@@ -41,18 +53,6 @@
     <t>Data7</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>URLs</t>
   </si>
   <si>
@@ -240,13 +240,49 @@
   </si>
   <si>
     <t>You’re temporarily logged in as Analyzer User. To switch back to your account, click on the icon at the bottom left of your screen.</t>
+  </si>
+  <si>
+    <t>Schedule Schema Incremental load</t>
+  </si>
+  <si>
+    <t>SchemaLoadJobDescription</t>
+  </si>
+  <si>
+    <t>SchemaLoadJobType</t>
+  </si>
+  <si>
+    <t>Incremental</t>
+  </si>
+  <si>
+    <t>SchemaLoadJobDate</t>
+  </si>
+  <si>
+    <t>12/31/2020</t>
+  </si>
+  <si>
+    <t>SchemaLoadJobTime</t>
+  </si>
+  <si>
+    <t>11:41 AM</t>
+  </si>
+  <si>
+    <t>SchemaLoadJobTimeZone</t>
+  </si>
+  <si>
+    <t>GMT+02:00</t>
+  </si>
+  <si>
+    <t>SchemaLoadJobRecurrence</t>
+  </si>
+  <si>
+    <t>No Recurrence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -269,9 +305,6 @@
       <sz val="11.0"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <color rgb="FF454545"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -293,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border/>
     <border>
       <left/>
@@ -315,19 +348,22 @@
       <top/>
       <bottom/>
     </border>
+    <border>
+      <bottom/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -360,8 +396,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,37 +437,37 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -1059,17 +1096,230 @@
       <c r="A29" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="9"/>
+      <c r="Z30" s="9"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="9"/>
+      <c r="Z32" s="9"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="9"/>
+      <c r="X33" s="9"/>
+      <c r="Y33" s="9"/>
+      <c r="Z33" s="9"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="9"/>
+      <c r="U34" s="9"/>
+      <c r="V34" s="9"/>
+      <c r="W34" s="9"/>
+      <c r="X34" s="9"/>
+      <c r="Y34" s="9"/>
+      <c r="Z34" s="9"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9"/>
+      <c r="W35" s="9"/>
+      <c r="X35" s="9"/>
+      <c r="Y35" s="9"/>
+      <c r="Z35" s="9"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="9"/>
+      <c r="V36" s="9"/>
+      <c r="W36" s="9"/>
+      <c r="X36" s="9"/>
+      <c r="Y36" s="9"/>
+      <c r="Z36" s="9"/>
+    </row>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
@@ -2035,13 +2285,14 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A30:C30"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2065,79 +2316,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Comments applied Element Names Updated function Names updated Added Folder/Files to git-ignore file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security/TestData.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFarid\git\qa\src\test\resources\TestDataFiles\security\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4880724E-EDF8-4B52-BE54-61813F88A58C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="TestData" sheetId="1" r:id="rId3"/>
-    <sheet state="hidden" name="Lists" sheetId="2" r:id="rId4"/>
+    <sheet name="TestData" sheetId="1" r:id="rId1"/>
+    <sheet name="Lists" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t>Supported Browser Types</t>
   </si>
@@ -128,60 +137,12 @@
     <t>Username</t>
   </si>
   <si>
-    <t>AbdelsalamAnalyzer</t>
-  </si>
-  <si>
-    <t>AbdelsalamIndividual</t>
-  </si>
-  <si>
-    <t>AbdelsalamSchemaManager</t>
-  </si>
-  <si>
-    <t>AbdelsalamUser</t>
-  </si>
-  <si>
-    <t>AbdelsalamUserManager</t>
-  </si>
-  <si>
-    <t>AbdelsalamSuper</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>farid</t>
-  </si>
-  <si>
-    <t>ahmed</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>AbdelsalamAnalyzer1</t>
-  </si>
-  <si>
-    <t>AbdelsalamIndividual1</t>
-  </si>
-  <si>
-    <t>AbdelsalamSchemaManager1</t>
-  </si>
-  <si>
-    <t>AbdelsalamUser1</t>
-  </si>
-  <si>
-    <t>AbdelsalamUserManager1</t>
-  </si>
-  <si>
-    <t>AbdelsalamSuper1</t>
-  </si>
-  <si>
-    <t>farid1</t>
-  </si>
-  <si>
-    <t>ahmed1</t>
-  </si>
-  <si>
     <t>Create DataSource</t>
   </si>
   <si>
@@ -294,33 +255,60 @@
   </si>
   <si>
     <t>No Recurrence</t>
+  </si>
+  <si>
+    <t>Automation_User_AnalyzerUser</t>
+  </si>
+  <si>
+    <t>Automation_User_IndividualAnalyzerUser</t>
+  </si>
+  <si>
+    <t>Automation_User_SchemaManagerUser</t>
+  </si>
+  <si>
+    <t>Automation_User_NormalUser</t>
+  </si>
+  <si>
+    <t>Automation_User_UserManagerUser</t>
+  </si>
+  <si>
+    <t>Automation_User_SuperUser3</t>
+  </si>
+  <si>
+    <t>Automation_User_SuperUser1</t>
+  </si>
+  <si>
+    <t>Automation_User_SuperUser2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -329,7 +317,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -345,116 +333,410 @@
     </fill>
   </fills>
   <borders count="6">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.86"/>
-    <col customWidth="1" min="2" max="2" width="26.43"/>
-    <col customWidth="1" min="3" max="3" width="27.14"/>
-    <col customWidth="1" min="4" max="4" width="30.0"/>
-    <col customWidth="1" min="5" max="6" width="28.29"/>
-    <col customWidth="1" min="7" max="7" width="28.86"/>
-    <col customWidth="1" min="8" max="15" width="8.57"/>
-    <col customWidth="1" min="16" max="17" width="8.71"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" customWidth="1"/>
+    <col min="10" max="15" width="8.5703125" customWidth="1"/>
+    <col min="16" max="17" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customHeight="1">
+    <row r="1" spans="1:17" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -491,881 +773,881 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-    </row>
-    <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-    </row>
-    <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-    </row>
-    <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-    </row>
-    <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-    </row>
-    <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-    </row>
-    <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-    </row>
-    <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="8" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-    </row>
-    <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="8" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-    </row>
-    <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-    </row>
-    <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="4" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+    </row>
+    <row r="12" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-    </row>
-    <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="7" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-    </row>
-    <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="7" t="s">
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="I14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="B15" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="1:26" ht="13.5" customHeight="1">
+      <c r="A17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="1:26" ht="13.5" customHeight="1">
+      <c r="A18" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="B18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="C18" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-    </row>
-    <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="7" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+    </row>
+    <row r="19" spans="1:26" ht="13.5" customHeight="1">
+      <c r="A19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+    </row>
+    <row r="20" spans="1:26" ht="13.5" customHeight="1">
+      <c r="A20" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="B20" s="6">
+        <v>30</v>
+      </c>
+      <c r="C20" s="6">
+        <v>30</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+    </row>
+    <row r="21" spans="1:26" ht="13.5" customHeight="1">
+      <c r="A21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+    </row>
+    <row r="22" spans="1:26" ht="13.5" customHeight="1">
+      <c r="A22" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="10" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+    </row>
+    <row r="23" spans="1:26" ht="13.5" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="B23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+    </row>
+    <row r="24" spans="1:26" ht="13.5" customHeight="1">
+      <c r="A24" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-    </row>
-    <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="11" t="s">
+      <c r="B24" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-    </row>
-    <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="8" t="s">
+      <c r="C24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+    </row>
+    <row r="25" spans="1:26" ht="13.5" customHeight="1">
+      <c r="A25" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+    </row>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A26" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="B26" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-    </row>
-    <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="8" t="s">
+      <c r="C26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+    </row>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A27" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A28" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-    </row>
-    <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="8" t="s">
+      <c r="B28" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A29" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-    </row>
-    <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="8" t="s">
+      <c r="B29" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="8">
-        <v>30.0</v>
-      </c>
-      <c r="C20" s="8">
-        <v>30.0</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-    </row>
-    <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="8" t="s">
+    </row>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A30" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B30" s="13"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+    </row>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A31" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A32" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-    </row>
-    <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="11" t="s">
+      <c r="B32" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-    </row>
-    <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="8" t="s">
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+    </row>
+    <row r="33" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A33" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-    </row>
-    <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="8" t="s">
+      <c r="B33" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+    </row>
+    <row r="34" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A34" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-    </row>
-    <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="11" t="s">
+      <c r="B34" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="8" t="s">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+    </row>
+    <row r="35" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A35" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B35" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A36" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="11" t="s">
+      <c r="B36" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" s="13"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
-      <c r="X30" s="9"/>
-      <c r="Y30" s="9"/>
-      <c r="Z30" s="9"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="9"/>
-      <c r="Y31" s="9"/>
-      <c r="Z31" s="9"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
-      <c r="X33" s="9"/>
-      <c r="Y33" s="9"/>
-      <c r="Z33" s="9"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
-      <c r="R34" s="9"/>
-      <c r="S34" s="9"/>
-      <c r="T34" s="9"/>
-      <c r="U34" s="9"/>
-      <c r="V34" s="9"/>
-      <c r="W34" s="9"/>
-      <c r="X34" s="9"/>
-      <c r="Y34" s="9"/>
-      <c r="Z34" s="9"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="9"/>
-      <c r="Y35" s="9"/>
-      <c r="Z35" s="9"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
-      <c r="T36" s="9"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="9"/>
-      <c r="W36" s="9"/>
-      <c r="X36" s="9"/>
-      <c r="Y36" s="9"/>
-      <c r="Z36" s="9"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
+    </row>
+    <row r="37" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="38" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="39" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="40" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="42" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -2320,36 +2602,32 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A30:C30"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A30:C30"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.29"/>
-    <col customWidth="1" min="2" max="11" width="8.57"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="11" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2364,7 +2642,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2379,7 +2657,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2394,7 +2672,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2409,7 +2687,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -3405,9 +3683,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating data files for legacy execution on scheduler/security
url should end with incorta/
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security/TestData.xlsx
@@ -59,55 +59,55 @@
     <t xml:space="preserve">URL_login_login</t>
   </si>
   <si>
-    <t xml:space="preserve">login</t>
+    <t xml:space="preserve">#/login</t>
   </si>
   <si>
     <t xml:space="preserve">URL_content_allContent</t>
   </si>
   <si>
-    <t xml:space="preserve">all-content/0</t>
+    <t xml:space="preserve">legacy/#/all-content/0</t>
   </si>
   <si>
     <t xml:space="preserve">URL_security_groups</t>
   </si>
   <si>
-    <t xml:space="preserve">security/groups</t>
+    <t xml:space="preserve">#/~/security/groups</t>
   </si>
   <si>
     <t xml:space="preserve">URL_security_users</t>
   </si>
   <si>
-    <t xml:space="preserve">security/users</t>
+    <t xml:space="preserve">#/~/security/users</t>
   </si>
   <si>
     <t xml:space="preserve">URL_data_dataSources</t>
   </si>
   <si>
-    <t xml:space="preserve">datasources/datasource</t>
+    <t xml:space="preserve">#/~/datasources/datasource</t>
   </si>
   <si>
     <t xml:space="preserve">URL_data_dataFiles</t>
   </si>
   <si>
-    <t xml:space="preserve">datasources/dataFiles</t>
+    <t xml:space="preserve">#/~/datasources/dataFiles</t>
   </si>
   <si>
     <t xml:space="preserve">URL_schemas_schemaList</t>
   </si>
   <si>
-    <t xml:space="preserve">schemas/schema-list</t>
+    <t xml:space="preserve">#/~/schemas/schema-list</t>
   </si>
   <si>
     <t xml:space="preserve">URL_scheduler_schemas</t>
   </si>
   <si>
-    <t xml:space="preserve">schedulers/scheduler-schemas</t>
+    <t xml:space="preserve">#/~/schedulers/scheduler-schemas</t>
   </si>
   <si>
     <t xml:space="preserve">URL_scheduler_dashboards</t>
   </si>
   <si>
-    <t xml:space="preserve">schedulers/scheduler-dashboards</t>
+    <t xml:space="preserve">#/~/schedulers/scheduler-dashboards</t>
   </si>
   <si>
     <t xml:space="preserve">User Credentials Analyzer</t>
@@ -506,19 +506,19 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="109.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="26.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="9.14"/>
   </cols>
@@ -2420,7 +2420,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.43"/>
   </cols>

</xml_diff>

<commit_message>
Revert "updating data files for legacy execution on scheduler/security"
This reverts commit ba88df15cc98ddb843f8f520a8d2b2d4e14114e3.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security/TestData.xlsx
@@ -59,55 +59,55 @@
     <t xml:space="preserve">URL_login_login</t>
   </si>
   <si>
-    <t xml:space="preserve">#/login</t>
+    <t xml:space="preserve">login</t>
   </si>
   <si>
     <t xml:space="preserve">URL_content_allContent</t>
   </si>
   <si>
-    <t xml:space="preserve">legacy/#/all-content/0</t>
+    <t xml:space="preserve">all-content/0</t>
   </si>
   <si>
     <t xml:space="preserve">URL_security_groups</t>
   </si>
   <si>
-    <t xml:space="preserve">#/~/security/groups</t>
+    <t xml:space="preserve">security/groups</t>
   </si>
   <si>
     <t xml:space="preserve">URL_security_users</t>
   </si>
   <si>
-    <t xml:space="preserve">#/~/security/users</t>
+    <t xml:space="preserve">security/users</t>
   </si>
   <si>
     <t xml:space="preserve">URL_data_dataSources</t>
   </si>
   <si>
-    <t xml:space="preserve">#/~/datasources/datasource</t>
+    <t xml:space="preserve">datasources/datasource</t>
   </si>
   <si>
     <t xml:space="preserve">URL_data_dataFiles</t>
   </si>
   <si>
-    <t xml:space="preserve">#/~/datasources/dataFiles</t>
+    <t xml:space="preserve">datasources/dataFiles</t>
   </si>
   <si>
     <t xml:space="preserve">URL_schemas_schemaList</t>
   </si>
   <si>
-    <t xml:space="preserve">#/~/schemas/schema-list</t>
+    <t xml:space="preserve">schemas/schema-list</t>
   </si>
   <si>
     <t xml:space="preserve">URL_scheduler_schemas</t>
   </si>
   <si>
-    <t xml:space="preserve">#/~/schedulers/scheduler-schemas</t>
+    <t xml:space="preserve">schedulers/scheduler-schemas</t>
   </si>
   <si>
     <t xml:space="preserve">URL_scheduler_dashboards</t>
   </si>
   <si>
-    <t xml:space="preserve">#/~/schedulers/scheduler-dashboards</t>
+    <t xml:space="preserve">schedulers/scheduler-dashboards</t>
   </si>
   <si>
     <t xml:space="preserve">User Credentials Analyzer</t>
@@ -506,19 +506,19 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="109.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="26.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="9.14"/>
   </cols>
@@ -2420,7 +2420,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.43"/>
   </cols>

</xml_diff>

<commit_message>
updating engine and testdata files for scheduler and security
url should end with incorta/
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security/TestData.xlsx
@@ -506,19 +506,19 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="109.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="26.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="9.14"/>
   </cols>
@@ -2420,7 +2420,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.43"/>
   </cols>

</xml_diff>